<commit_message>
Set up for running more flexible number of years
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24_age1srv.xlsx
+++ b/data/hake_input_yr24_age1srv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DDD5C-A55C-6446-A89C-D04E40380064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F3D3C9-A7C6-804B-B1D4-3E1C21C51EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="6100" windowWidth="34420" windowHeight="33040" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="5540" windowWidth="34420" windowHeight="33040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1613,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2562,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
@@ -27519,10 +27519,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27535,9 +27535,9 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1980</v>
+        <v>1966</v>
       </c>
       <c r="B2" s="3">
         <v>7.7910786500000002</v>
@@ -27545,345 +27545,457 @@
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1981</v>
+        <v>1967</v>
       </c>
       <c r="B3" s="3">
-        <v>7.9302527500000002</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1982</v>
+        <v>1968</v>
       </c>
       <c r="B4" s="3">
-        <v>7.7663626399999997</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1983</v>
+        <v>1969</v>
       </c>
       <c r="B5" s="3">
-        <v>8.3381739100000001</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1984</v>
+        <v>1970</v>
       </c>
       <c r="B6" s="3">
-        <v>7.7257362599999997</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1985</v>
+        <v>1971</v>
       </c>
       <c r="B7" s="3">
-        <v>7.5189010999999999</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1986</v>
+        <v>1972</v>
       </c>
       <c r="B8" s="3">
-        <v>7.7015434799999998</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1987</v>
+        <v>1973</v>
       </c>
       <c r="B9" s="3">
-        <v>7.9614065900000002</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1988</v>
+        <v>1974</v>
       </c>
       <c r="B10" s="3">
-        <v>7.54096703</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1989</v>
+        <v>1975</v>
       </c>
       <c r="B11" s="3">
-        <v>7.4454456499999999</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1990</v>
+        <v>1976</v>
       </c>
       <c r="B12" s="3">
-        <v>7.6304835200000003</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1991</v>
+        <v>1977</v>
       </c>
       <c r="B13" s="3">
-        <v>7.3921977999999999</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1992</v>
+        <v>1978</v>
       </c>
       <c r="B14" s="3">
-        <v>8.0989565199999998</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1993</v>
+        <v>1979</v>
       </c>
       <c r="B15" s="3">
-        <v>7.6743296699999997</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1994</v>
+        <v>1980</v>
       </c>
       <c r="B16" s="3">
-        <v>7.6574285700000004</v>
+        <v>7.7910786500000002</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1995</v>
+        <v>1981</v>
       </c>
       <c r="B17" s="3">
-        <v>7.7381758200000004</v>
+        <v>7.9302527500000002</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1996</v>
+        <v>1982</v>
       </c>
       <c r="B18" s="3">
-        <v>7.7203152199999998</v>
+        <v>7.7663626399999997</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1997</v>
+        <v>1983</v>
       </c>
       <c r="B19" s="3">
-        <v>8.1091318700000006</v>
+        <v>8.3381739100000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1998</v>
+        <v>1984</v>
       </c>
       <c r="B20" s="3">
-        <v>8.1201428599999996</v>
+        <v>7.7257362599999997</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1999</v>
+        <v>1985</v>
       </c>
       <c r="B21" s="3">
-        <v>7.33834783</v>
+        <v>7.5189010999999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2000</v>
+        <v>1986</v>
       </c>
       <c r="B22" s="3">
-        <v>7.4241428599999999</v>
+        <v>7.7015434799999998</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2001</v>
+        <v>1987</v>
       </c>
       <c r="B23" s="3">
-        <v>7.0958131900000003</v>
+        <v>7.9614065900000002</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2002</v>
+        <v>1988</v>
       </c>
       <c r="B24" s="3">
-        <v>7.2639239099999999</v>
+        <v>7.54096703</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2003</v>
+        <v>1989</v>
       </c>
       <c r="B25" s="3">
-        <v>7.5445054899999997</v>
+        <v>7.4454456499999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2004</v>
+        <v>1990</v>
       </c>
       <c r="B26" s="3">
-        <v>7.64548352</v>
+        <v>7.6304835200000003</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2005</v>
+        <v>1991</v>
       </c>
       <c r="B27" s="3">
-        <v>7.8828369599999997</v>
+        <v>7.3921977999999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2006</v>
+        <v>1992</v>
       </c>
       <c r="B28" s="3">
-        <v>7.7766813199999998</v>
+        <v>8.0989565199999998</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2007</v>
+        <v>1993</v>
       </c>
       <c r="B29" s="3">
-        <v>7.4721978</v>
+        <v>7.6743296699999997</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2008</v>
+        <v>1994</v>
       </c>
       <c r="B30" s="3">
-        <v>7.1410434800000004</v>
+        <v>7.6574285700000004</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2009</v>
+        <v>1995</v>
       </c>
       <c r="B31" s="3">
-        <v>7.20131868</v>
+        <v>7.7381758200000004</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2010</v>
+        <v>1996</v>
       </c>
       <c r="B32" s="3">
-        <v>7.4271111100000002</v>
+        <v>7.7203152199999998</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2011</v>
+        <v>1997</v>
       </c>
       <c r="B33" s="3">
-        <v>7.4726153799999997</v>
+        <v>8.1091318700000006</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2012</v>
+        <v>1998</v>
       </c>
       <c r="B34" s="3">
-        <v>7.2943695699999997</v>
+        <v>8.1201428599999996</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2013</v>
+        <v>1999</v>
       </c>
       <c r="B35" s="3">
-        <v>7.0181098899999999</v>
+        <v>7.33834783</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2014</v>
+        <v>2000</v>
       </c>
       <c r="B36" s="3">
-        <v>7.4749340699999998</v>
+        <v>7.4241428599999999</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2015</v>
+        <v>2001</v>
       </c>
       <c r="B37" s="3">
-        <v>7.5457142900000003</v>
+        <v>7.0958131900000003</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2016</v>
+        <v>2002</v>
       </c>
       <c r="B38" s="3">
-        <v>7.3323152199999999</v>
+        <v>7.2639239099999999</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2017</v>
+        <v>2003</v>
       </c>
       <c r="B39" s="3">
-        <v>7.3101318700000002</v>
+        <v>7.5445054899999997</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2018</v>
+        <v>2004</v>
       </c>
       <c r="B40" s="3">
-        <v>7.4305384600000002</v>
+        <v>7.64548352</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>2019</v>
+        <v>2005</v>
       </c>
       <c r="B41" s="3">
-        <v>7.3799565200000004</v>
+        <v>7.8828369599999997</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2020</v>
+        <v>2006</v>
       </c>
       <c r="B42" s="3">
-        <v>7.3799565200000004</v>
+        <v>7.7766813199999998</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2021</v>
+        <v>2007</v>
       </c>
       <c r="B43" s="3">
-        <v>7.3799565200000004</v>
+        <v>7.4721978</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>2022</v>
+        <v>2008</v>
       </c>
       <c r="B44" s="3">
-        <v>7.3799565200000004</v>
+        <v>7.1410434800000004</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A45">
+        <v>2009</v>
+      </c>
+      <c r="B45" s="3">
+        <v>7.20131868</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2010</v>
+      </c>
+      <c r="B46" s="3">
+        <v>7.4271111100000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2011</v>
+      </c>
+      <c r="B47" s="3">
+        <v>7.4726153799999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2012</v>
+      </c>
+      <c r="B48" s="3">
+        <v>7.2943695699999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2013</v>
+      </c>
+      <c r="B49" s="3">
+        <v>7.0181098899999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2014</v>
+      </c>
+      <c r="B50" s="3">
+        <v>7.4749340699999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2015</v>
+      </c>
+      <c r="B51" s="3">
+        <v>7.5457142900000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2016</v>
+      </c>
+      <c r="B52" s="3">
+        <v>7.3323152199999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2017</v>
+      </c>
+      <c r="B53" s="3">
+        <v>7.3101318700000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2018</v>
+      </c>
+      <c r="B54" s="3">
+        <v>7.4305384600000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2019</v>
+      </c>
+      <c r="B55" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2020</v>
+      </c>
+      <c r="B56" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2021</v>
+      </c>
+      <c r="B57" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2022</v>
+      </c>
+      <c r="B58" s="3">
+        <v>7.3799565200000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59">
         <v>2023</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B59" s="3">
         <v>7.3799565200000004</v>
       </c>
     </row>
@@ -32108,8 +32220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37297,7 +37409,7 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="D2" sqref="D2:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Tweaked selectivity, sigma R prior, etc.
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24_age1srv.xlsx
+++ b/data/hake_input_yr24_age1srv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F3D3C9-A7C6-804B-B1D4-3E1C21C51EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF575DA-9616-B947-829E-2553BC0363AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="5540" windowWidth="34420" windowHeight="33040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43460" yWindow="17140" windowWidth="30260" windowHeight="21340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4035,7 +4035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y295"/>
   <sheetViews>
-    <sheetView topLeftCell="A213" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A253" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P298" sqref="P298"/>
     </sheetView>
   </sheetViews>
@@ -32220,8 +32220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32344,7 +32344,7 @@
         <v>61</v>
       </c>
       <c r="B15">
-        <v>1.24</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -35345,8 +35345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35489,7 +35489,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1.4</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -35575,7 +35575,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>7.5499999999999998E-2</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -35601,7 +35601,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -35649,7 +35649,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>7.5499999999999998E-2</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -45340,7 +45340,7 @@
   <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Y110"/>
+      <selection activeCell="A2" sqref="A2:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Corrected parameterization of age-1 index
</commit_message>
<xml_diff>
--- a/data/hake_input_yr24_age1srv.xlsx
+++ b/data/hake_input_yr24_age1srv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8E92AB-9DDD-A949-B8DD-D9866576688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89365F5-6286-954A-86C0-62A8E3C78AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="8000" windowWidth="54680" windowHeight="35200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21080" yWindow="1680" windowWidth="35340" windowHeight="32160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="396">
   <si>
     <t>Number</t>
   </si>
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35225,8 +35225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35481,10 +35481,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -35496,7 +35496,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -35514,7 +35514,7 @@
         <v>1</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q4">
         <v>3</v>
@@ -45205,10 +45205,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -45297,6 +45297,83 @@
       </c>
       <c r="Y1" s="1" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>